<commit_message>
add the supplement directory
</commit_message>
<xml_diff>
--- a/SRC/Simulation/InformationTable.xlsx
+++ b/SRC/Simulation/InformationTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Automata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="259">
   <si>
     <t>Automata Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -861,6 +861,38 @@
   </si>
   <si>
     <t>0 means this superstate is not in the BDD supervisor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Withdrawal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Navigation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fuel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drogue&amp;probe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Datalink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TankerSafety</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1392,7 +1424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -5193,8 +5225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q236"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5206,21 +5238,37 @@
       <c r="A1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>255</v>
+      </c>
       <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
+      <c r="L1" s="7" t="s">
+        <v>256</v>
+      </c>
       <c r="M1" s="7"/>
-      <c r="N1" s="8"/>
+      <c r="N1" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
+      <c r="P1" s="9" t="s">
+        <v>258</v>
+      </c>
       <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -17681,6 +17729,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>